<commit_message>
Update data presentation with overview
</commit_message>
<xml_diff>
--- a/0_data/0-raw/FRANCE/variables.xlsx
+++ b/0_data/0-raw/FRANCE/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://technip.sharepoint.com/sites/DUP-2023-2024-CO2emission/Shared Documents/🌍CO2 emission/4-CNs/0-Raw data/FRANCE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rmarinho\Desktop\REGINALDO\0-TP\13-Data Science DUP\8-Project\CO2EmissionsDUP\0_data\0-raw\FRANCE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{1020FD5B-84E1-4B77-A75D-F8C13F580F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A54BFAD-CE40-4580-B27C-0E7D3ED8502B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F5CC92-DFED-471F-BC6F-C385399E8FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15555" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28740" yWindow="-16455" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FR" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="129">
   <si>
     <t>nom-colonne</t>
   </si>
@@ -245,9 +245,6 @@
     <t>gamme</t>
   </si>
   <si>
-    <t>typerubric</t>
-  </si>
-  <si>
     <t>length</t>
   </si>
   <si>
@@ -444,6 +441,12 @@
   </si>
   <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>type</t>
   </si>
 </sst>
 </file>
@@ -551,10 +554,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1308,7 +1307,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,19 +1321,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,7 +1347,7 @@
         <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1362,7 +1361,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1376,7 +1375,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1390,7 +1389,7 @@
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1404,7 +1403,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1418,7 +1417,7 @@
         <v>36</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,7 +1431,7 @@
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,7 +1445,7 @@
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1460,7 +1459,7 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,7 +1473,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
@@ -1491,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1505,10 +1504,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1522,10 +1521,10 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1539,10 +1538,10 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,10 +1555,10 @@
         <v>3</v>
       </c>
       <c r="D16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" t="s">
         <v>74</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -1573,10 +1572,10 @@
         <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -1590,10 +1589,10 @@
         <v>11</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -1607,10 +1606,10 @@
         <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -1624,10 +1623,10 @@
         <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1662,10 +1661,10 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -1679,7 +1678,7 @@
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
         <v>52</v>
@@ -1696,7 +1695,7 @@
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E23" t="s">
         <v>52</v>
@@ -1713,7 +1712,7 @@
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -1727,7 +1726,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -1741,7 +1740,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
@@ -1755,7 +1754,7 @@
         <v>14</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1768,7 @@
   <dimension ref="A1:Y27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1785,16 +1784,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E1" s="6">
         <v>2015</v>
@@ -1825,22 +1824,22 @@
         <v>The brand</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>89</v>
-      </c>
       <c r="H2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1855,7 +1854,7 @@
         <v>The file model</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>8</v>
@@ -1864,7 +1863,7 @@
         <v>8</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>8</v>
@@ -1885,16 +1884,16 @@
         <v>The business model</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>10</v>
@@ -1915,7 +1914,7 @@
         <v>Commercial designation</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>12</v>
@@ -1924,7 +1923,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>12</v>
@@ -1945,7 +1944,7 @@
         <v>The National Type Identification Code (CNIT)</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>14</v>
@@ -1954,7 +1953,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>14</v>
@@ -1975,7 +1974,7 @@
         <v>The Variant-Variant (TVV) or the Mines type</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>16</v>
@@ -1984,7 +1983,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>16</v>
@@ -2005,22 +2004,22 @@
         <v>The type of fuel</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="I8" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -2035,7 +2034,7 @@
         <v>Information to identify hybrid vehicles (O/N)</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>20</v>
@@ -2044,13 +2043,13 @@
         <v>20</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2065,16 +2064,16 @@
         <v>Administrative power</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>22</v>
@@ -2104,7 +2103,7 @@
         <v>25</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>25</v>
@@ -2125,7 +2124,7 @@
         <v>The type of gearbox and the number of reports,</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>28</v>
@@ -2134,7 +2133,7 @@
         <v>28</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>28</v>
@@ -2155,16 +2154,16 @@
         <v>Urban fuel consumption (in L/100km),</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>30</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>30</v>
@@ -2185,7 +2184,7 @@
         <v>Mixed fuel consumption (in L/100km),</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>33</v>
@@ -2194,7 +2193,7 @@
         <v>33</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H14" s="4" t="s">
         <v>33</v>
@@ -2215,7 +2214,7 @@
         <v>Extra urban fuel consumption (in L/100km),</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>35</v>
@@ -2224,7 +2223,7 @@
         <v>35</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>35</v>
@@ -2245,16 +2244,16 @@
         <v>CO2 emission (in G/km),</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>37</v>
@@ -2275,7 +2274,7 @@
         <v>CO Type I test result</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>40</v>
@@ -2284,13 +2283,13 @@
         <v>40</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -2305,7 +2304,7 @@
         <v>Results of test HC</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>42</v>
@@ -2314,13 +2313,13 @@
         <v>42</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -2335,7 +2334,7 @@
         <v>Nox trial results</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>44</v>
@@ -2344,13 +2343,13 @@
         <v>44</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>44</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -2365,7 +2364,7 @@
         <v>HC+Nox trial results</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>46</v>
@@ -2374,13 +2373,13 @@
         <v>46</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>46</v>
       </c>
       <c r="I20" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -2411,7 +2410,7 @@
         <v>particle test result</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>48</v>
@@ -2420,13 +2419,13 @@
         <v>48</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>48</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2450,13 +2449,13 @@
         <v>50</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="I22" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -2480,13 +2479,13 @@
         <v>53</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>53</v>
       </c>
       <c r="I23" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2501,7 +2500,7 @@
         <v>Field V9 of the registration certificate which contains the Euro standard</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>55</v>
@@ -2510,7 +2509,7 @@
         <v>55</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H24" s="4" t="s">
         <v>55</v>
@@ -2531,7 +2530,7 @@
         <v>The date of the last update.</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>57</v>
@@ -2540,7 +2539,7 @@
         <v>57</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>57</v>
@@ -2561,10 +2560,10 @@
         <v>Body</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F26" s="4" t="s">
         <v>59</v>
@@ -2576,7 +2575,7 @@
         <v>59</v>
       </c>
       <c r="I26" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -2591,10 +2590,10 @@
         <v>Range</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F27" s="4" t="s">
         <v>60</v>
@@ -2606,7 +2605,7 @@
         <v>60</v>
       </c>
       <c r="I27" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2621,15 +2620,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="e5576a18-6290-466e-96c3-a3c8a1587d46">
@@ -2637,6 +2627,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2812,19 +2811,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26235964-1ECE-4E44-9FA6-52C82DA2DBFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1219E20-8E10-456B-A9B3-8B456B18A0DA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e5576a18-6290-466e-96c3-a3c8a1587d46"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1219E20-8E10-456B-A9B3-8B456B18A0DA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26235964-1ECE-4E44-9FA6-52C82DA2DBFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e5576a18-6290-466e-96c3-a3c8a1587d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2845,4 +2844,10 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{b29603fb-7fab-4bf6-8ed3-004985bb9d91}" enabled="1" method="Standard" siteId="{9179d01a-e94c-4488-b5f0-4554bc474f8c}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>